<commit_message>
toymaker example in 3 types of code
added toymaker example with 3 types of code.
</commit_message>
<xml_diff>
--- a/linear-programming/excel/Excel-Solver-Example-LP.xlsx
+++ b/linear-programming/excel/Excel-Solver-Example-LP.xlsx
@@ -8,49 +8,52 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RobertH/Documents/GitHub/open-optimization-or-examples/linear-programming/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{766EA43E-0D92-4049-9308-ADFBED983934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8B6A71-534A-604C-AF33-46463F84BCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39860" yWindow="-40" windowWidth="20620" windowHeight="16900" xr2:uid="{89BC7A85-BA86-3840-90D3-305A87FE491D}"/>
+    <workbookView xWindow="8600" yWindow="1500" windowWidth="20620" windowHeight="16900" activeTab="3" xr2:uid="{89BC7A85-BA86-3840-90D3-305A87FE491D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Optimization Model" sheetId="1" r:id="rId1"/>
-    <sheet name="Answer Report 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sensitivity Report 1" sheetId="3" r:id="rId3"/>
-    <sheet name="Limits Report 1" sheetId="4" r:id="rId4"/>
+    <sheet name="Answer Report 2" sheetId="5" r:id="rId1"/>
+    <sheet name="Sensitivity Report 2" sheetId="6" r:id="rId2"/>
+    <sheet name="Limits Report 2" sheetId="7" r:id="rId3"/>
+    <sheet name="Optimization Model" sheetId="1" r:id="rId4"/>
+    <sheet name="Answer Report 1" sheetId="2" r:id="rId5"/>
+    <sheet name="Sensitivity Report 1" sheetId="3" r:id="rId6"/>
+    <sheet name="Limits Report 1" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Optimization Model'!$C$8:$G$8</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Optimization Model'!$H$11:$H$12</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Optimization Model'!$H$13:$H$14</definedName>
-    <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Optimization Model'!$C$5</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Optimization Model'!$J$11:$J$12</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Optimization Model'!$J$13:$J$14</definedName>
-    <definedName name="solver_rlx" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'Optimization Model'!$C$8:$G$8</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Optimization Model'!$H$11:$H$12</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Optimization Model'!$H$13:$H$14</definedName>
+    <definedName name="solver_lin" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'Optimization Model'!$C$5</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'Optimization Model'!$J$11:$J$12</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'Optimization Model'!$J$13:$J$14</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -69,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="88">
   <si>
     <t>variables</t>
   </si>
@@ -312,6 +315,27 @@
   </si>
   <si>
     <t>Upper</t>
+  </si>
+  <si>
+    <t>Worksheet: [Excel-Solver-Example-LP.xlsx]Optimization Model</t>
+  </si>
+  <si>
+    <t>Report Created: 1/27/22 10:37:00 PM</t>
+  </si>
+  <si>
+    <t>Solution Time: 4295291.228 Seconds.</t>
+  </si>
+  <si>
+    <t>Iterations: 3 Subproblems: 0</t>
+  </si>
+  <si>
+    <t>Max Time Unlimited, Iterations Unlimited, Precision 0.000001</t>
+  </si>
+  <si>
+    <t>Not Binding</t>
+  </si>
+  <si>
+    <t>Report Created: 1/27/22 10:37:01 PM</t>
   </si>
 </sst>
 </file>
@@ -860,11 +884,948 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF9085F-545E-A546-B717-40C20E127EB7}">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" collapsed="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="13">
+        <v>172706.33333333331</v>
+      </c>
+      <c r="E16" s="13">
+        <v>252000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="14">
+        <v>11336.666666666666</v>
+      </c>
+      <c r="E22" s="14">
+        <v>18000</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="14">
+        <v>666.33333333333326</v>
+      </c>
+      <c r="E23" s="14">
+        <v>0</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="14">
+        <v>16004</v>
+      </c>
+      <c r="E24" s="14">
+        <v>24000</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="14">
+        <v>0</v>
+      </c>
+      <c r="E25" s="14">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="13">
+        <v>4001</v>
+      </c>
+      <c r="E26" s="13">
+        <v>6000</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="30" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="14">
+        <v>4000</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="14">
+        <v>6000</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="14">
+        <v>0</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="13">
+        <v>0</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3480FE15-2A74-F44F-8061-9A7D05D616F9}">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="12">
+        <v>18000</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12">
+        <v>7</v>
+      </c>
+      <c r="G10" s="12">
+        <v>1E+30</v>
+      </c>
+      <c r="H10" s="12">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12">
+        <v>-119</v>
+      </c>
+      <c r="F11" s="12">
+        <v>14</v>
+      </c>
+      <c r="G11" s="12">
+        <v>119</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="12">
+        <v>24000</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12">
+        <v>6</v>
+      </c>
+      <c r="G12" s="12">
+        <v>1E+30</v>
+      </c>
+      <c r="H12" s="12">
+        <v>8.8888888888888893</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12">
+        <v>-80</v>
+      </c>
+      <c r="F13" s="12">
+        <v>10</v>
+      </c>
+      <c r="G13" s="12">
+        <v>80</v>
+      </c>
+      <c r="H13" s="12">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9">
+        <v>6000</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>-3</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1E+30</v>
+      </c>
+      <c r="H14" s="9">
+        <v>39.666666666666664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="12">
+        <v>4000</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="12">
+        <v>4001</v>
+      </c>
+      <c r="G20" s="12">
+        <v>1E+30</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="12">
+        <v>6000</v>
+      </c>
+      <c r="E21" s="12">
+        <v>42</v>
+      </c>
+      <c r="F21" s="12">
+        <v>6000</v>
+      </c>
+      <c r="G21" s="12">
+        <v>1E+30</v>
+      </c>
+      <c r="H21" s="12">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12">
+        <v>7</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>1E+30</v>
+      </c>
+      <c r="H22" s="12">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>6</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>1E+30</v>
+      </c>
+      <c r="H23" s="9">
+        <v>24000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC56C30-6C3E-4F41-837B-758741BBDAA7}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="13">
+        <v>252000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="F11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="14">
+        <v>18000</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="14">
+        <v>85</v>
+      </c>
+      <c r="I14" s="14">
+        <v>250</v>
+      </c>
+      <c r="J14" s="14">
+        <v>18835</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0</v>
+      </c>
+      <c r="G15" s="14">
+        <v>110</v>
+      </c>
+      <c r="I15" s="14">
+        <v>398.5</v>
+      </c>
+      <c r="J15" s="14">
+        <v>20035</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="14">
+        <v>24000</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0</v>
+      </c>
+      <c r="G16" s="14">
+        <v>125</v>
+      </c>
+      <c r="I16" s="14">
+        <v>597</v>
+      </c>
+      <c r="J16" s="14">
+        <v>21020</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="2:10" ht="17" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="13">
+        <v>6000</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="2:10" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D440DB36-BAF8-8D46-B7B2-CBA8858E796D}">
   <dimension ref="A4:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,7 +1848,7 @@
       </c>
       <c r="C5" s="6">
         <f>SUMPRODUCT(C8:G8,C6:G6)</f>
-        <v>172666.66666666669</v>
+        <v>252000</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -920,19 +1881,19 @@
         <v>2</v>
       </c>
       <c r="C8" s="4">
-        <v>11333.333333333334</v>
+        <v>18000</v>
       </c>
       <c r="D8" s="4">
-        <v>666.66666666666663</v>
+        <v>0</v>
       </c>
       <c r="E8" s="4">
-        <v>16000</v>
+        <v>24000</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>15</v>
@@ -965,18 +1926,17 @@
         <v>1</v>
       </c>
       <c r="H11" s="1">
-        <f>SUMPRODUCT($C$8:$G$8,C11:G11)</f>
         <v>4000</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J11">
-        <v>4000</v>
+        <v>4001</v>
       </c>
       <c r="L11" s="1">
         <f>J11-H11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1075,7 +2035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56C753B-FC2D-5346-B9DC-D18AC524CEF8}">
   <dimension ref="A1:G35"/>
   <sheetViews>
@@ -1419,12 +2379,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C234E-ADAF-EC4D-8B0A-067412FB432D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1779,7 +2739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3045BFC7-DB8D-8A45-BAD2-05D057B1FFF3}">
   <dimension ref="A1:J19"/>
   <sheetViews>

</xml_diff>